<commit_message>
checked and updated conf.py, demo_lists.xlsx, and removed list_of_demos.rst
</commit_message>
<xml_diff>
--- a/demo_lists.xlsx
+++ b/demo_lists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/icaoberg/Desktop/cellorganizer-docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulaniqi/Desktop/CBD/gitlab_repos/cellorganizer-docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="18680" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="18680" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="v2.5" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
   </sheets>
   <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="81">
   <si>
     <t>Name</t>
   </si>
@@ -181,12 +184,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>demo2D05</t>
-  </si>
-  <si>
-    <t>img2param_2D</t>
-  </si>
-  <si>
     <t>surface plot</t>
   </si>
   <si>
@@ -272,6 +269,12 @@
   </si>
   <si>
     <t>demo3D43</t>
+  </si>
+  <si>
+    <t>demo3D44</t>
+  </si>
+  <si>
+    <t>demo3D45</t>
   </si>
 </sst>
 </file>
@@ -1625,11 +1628,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1828,42 +1831,39 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C7" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="D7" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="E7" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="F7" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G7" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H7" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I7" t="s">
-        <v>51</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
@@ -1895,7 +1895,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -1905,29 +1905,32 @@
         <v>0</v>
       </c>
       <c r="D9" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="E9" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="F9" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="G9" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H9" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -1937,32 +1940,29 @@
         <v>0</v>
       </c>
       <c r="D10" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="E10" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="F10" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G10" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H10" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I10" t="s">
-        <v>52</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -1988,13 +1988,13 @@
         <v>1</v>
       </c>
       <c r="H11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -2020,13 +2020,13 @@
         <v>1</v>
       </c>
       <c r="H12" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -2058,7 +2058,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -2090,7 +2090,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -2122,7 +2122,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
@@ -2154,7 +2154,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
@@ -2186,18 +2186,18 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
         <v>14</v>
       </c>
       <c r="C18" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="D18" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="E18" t="b">
         <f>FALSE()</f>
@@ -2218,7 +2218,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
@@ -2250,14 +2250,14 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
       </c>
       <c r="C20" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D20" t="b">
         <f>FALSE()</f>
@@ -2268,21 +2268,24 @@
         <v>0</v>
       </c>
       <c r="F20" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="G20" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H20" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
         <v>14</v>
@@ -2312,12 +2315,12 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
         <v>14</v>
@@ -2327,32 +2330,29 @@
         <v>0</v>
       </c>
       <c r="D22" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="E22" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="F22" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G22" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H22" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I22" t="s">
-        <v>54</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
         <v>14</v>
@@ -2362,36 +2362,39 @@
         <v>0</v>
       </c>
       <c r="D23" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="E23" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="F23" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="G23" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H23" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
         <v>14</v>
       </c>
       <c r="C24" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="D24" t="b">
         <f>FALSE()</f>
@@ -2402,31 +2405,28 @@
         <v>0</v>
       </c>
       <c r="F24" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G24" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H24" t="b">
         <f>FALSE()</f>
         <v>0</v>
-      </c>
-      <c r="I24" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
         <v>14</v>
       </c>
       <c r="C25" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D25" t="b">
         <f>FALSE()</f>
@@ -2437,56 +2437,56 @@
         <v>0</v>
       </c>
       <c r="F25" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="G25" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H25" t="b">
         <f>FALSE()</f>
         <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
         <v>14</v>
       </c>
       <c r="C26" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="D26" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E26" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="F26" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G26" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H26" t="b">
         <f>FALSE()</f>
         <v>0</v>
-      </c>
-      <c r="I26" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
         <v>14</v>
@@ -2500,8 +2500,8 @@
         <v>0</v>
       </c>
       <c r="E27" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="F27" t="b">
         <f>TRUE()</f>
@@ -2518,22 +2518,22 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
         <v>14</v>
       </c>
       <c r="C28" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D28" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="E28" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="F28" t="b">
         <f>TRUE()</f>
@@ -2544,13 +2544,13 @@
         <v>1</v>
       </c>
       <c r="H28" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B29" t="s">
         <v>14</v>
@@ -2564,8 +2564,8 @@
         <v>1</v>
       </c>
       <c r="E29" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="F29" t="b">
         <f>TRUE()</f>
@@ -2581,8 +2581,8 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>60</v>
+      <c r="A30" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="B30" t="s">
         <v>14</v>
@@ -2614,7 +2614,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
         <v>14</v>
@@ -2642,11 +2642,14 @@
       <c r="H31" t="b">
         <f>TRUE()</f>
         <v>1</v>
+      </c>
+      <c r="I31" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
         <v>14</v>
@@ -2660,8 +2663,8 @@
         <v>1</v>
       </c>
       <c r="E32" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="F32" t="b">
         <f>TRUE()</f>
@@ -2672,16 +2675,13 @@
         <v>1</v>
       </c>
       <c r="H32" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I32" t="s">
-        <v>57</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" t="s">
         <v>14</v>
@@ -2691,8 +2691,8 @@
         <v>0</v>
       </c>
       <c r="D33" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="E33" t="b">
         <f>TRUE()</f>
@@ -2709,11 +2709,14 @@
       <c r="H33" t="b">
         <f>FALSE()</f>
         <v>0</v>
+      </c>
+      <c r="I33" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" t="s">
         <v>14</v>
@@ -2727,76 +2730,65 @@
         <v>0</v>
       </c>
       <c r="E34" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="F34" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="G34" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H34" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" t="s">
         <v>14</v>
       </c>
       <c r="C35" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" t="b">
-        <f>FALSE()</f>
+        <f>NOT(C35)</f>
         <v>0</v>
       </c>
       <c r="E35" t="b">
-        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="F35" t="b">
-        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="G35" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H35" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I35" t="s">
-        <v>59</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B36" t="s">
         <v>14</v>
       </c>
       <c r="C36" t="b">
-        <v>1</v>
-      </c>
-      <c r="D36" t="b">
-        <f>NOT(C36)</f>
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="b">
+        <f t="shared" ref="D36:D49" si="0">NOT(C36)</f>
+        <v>1</v>
       </c>
       <c r="E36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
@@ -2807,36 +2799,27 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
       </c>
       <c r="D37" s="1" t="b">
-        <f t="shared" ref="D37:D50" si="0">NOT(C37)</f>
-        <v>1</v>
-      </c>
-      <c r="E37" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" t="b">
-        <v>0</v>
-      </c>
-      <c r="G37" t="b">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C38" t="b">
+      <c r="C38" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D38" s="1" t="b">
@@ -2846,7 +2829,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>14</v>
@@ -2861,7 +2844,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>14</v>
@@ -2876,7 +2859,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>14</v>
@@ -2891,7 +2874,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>14</v>
@@ -2906,7 +2889,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>14</v>
@@ -2921,7 +2904,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>14</v>
@@ -2936,7 +2919,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>14</v>
@@ -2951,77 +2934,90 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C46" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" s="1" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C47" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47" s="1" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C48" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" s="1" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C49" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49" s="1" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" t="b">
+        <v>0</v>
+      </c>
+      <c r="D50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>80</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D50" s="1" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="B51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced demo3D35 with demo3D47. Now there are 46 3D demos.
</commit_message>
<xml_diff>
--- a/demo_lists.xlsx
+++ b/demo_lists.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Multimedia/Code/cellorganizer-docs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27526"/>
+  <workbookPr autoCompressPictures="0"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="5360" yWindow="1240" windowWidth="25600" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="v2.5" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,7 @@
     <sheet name="v2.7.0" sheetId="3" r:id="rId3"/>
     <sheet name="v2.6" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -399,7 +394,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -434,7 +429,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -611,7 +606,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -626,9 +621,9 @@
       <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -651,7 +646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -679,7 +674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -707,7 +702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -735,7 +730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -763,7 +758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -791,7 +786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -819,7 +814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -847,7 +842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -875,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -903,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -931,7 +926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -959,7 +954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -987,7 +982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1015,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1043,7 +1038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1071,7 +1066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1099,7 +1094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1127,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1155,7 +1150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1183,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1211,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1239,7 +1234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1267,7 +1262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1295,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1323,7 +1318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1351,7 +1346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1379,7 +1374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1407,7 +1402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1435,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -1463,7 +1458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -1491,7 +1486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -1519,7 +1514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -1547,7 +1542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -1575,7 +1570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -1603,7 +1598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -1626,7 +1621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -1652,6 +1647,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1660,16 +1660,16 @@
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1702,7 +1702,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1721,7 +1721,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1740,7 +1740,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1759,7 +1759,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1778,7 +1778,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>81</v>
       </c>
@@ -1797,7 +1797,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>82</v>
       </c>
@@ -1816,7 +1816,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>83</v>
       </c>
@@ -1835,7 +1835,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>84</v>
       </c>
@@ -1854,7 +1854,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>85</v>
       </c>
@@ -1873,7 +1873,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1892,7 +1892,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -1911,7 +1911,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1930,7 +1930,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -1949,7 +1949,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1968,7 +1968,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1987,7 +1987,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -2006,7 +2006,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -2025,7 +2025,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -2044,7 +2044,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -2063,7 +2063,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -2082,7 +2082,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -2101,7 +2101,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -2120,7 +2120,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -2139,7 +2139,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -2158,7 +2158,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -2177,7 +2177,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -2196,7 +2196,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
@@ -2215,7 +2215,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -2234,7 +2234,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -2253,7 +2253,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -2272,7 +2272,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -2291,7 +2291,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
@@ -2310,7 +2310,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
@@ -2329,7 +2329,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
         <v>60</v>
       </c>
@@ -2348,7 +2348,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
         <v>61</v>
       </c>
@@ -2367,7 +2367,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
@@ -2386,7 +2386,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
         <v>63</v>
       </c>
@@ -2405,7 +2405,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
         <v>64</v>
       </c>
@@ -2424,7 +2424,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
         <v>65</v>
       </c>
@@ -2443,7 +2443,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
         <v>66</v>
       </c>
@@ -2462,7 +2462,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
         <v>67</v>
       </c>
@@ -2481,7 +2481,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
         <v>68</v>
       </c>
@@ -2500,7 +2500,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
         <v>69</v>
       </c>
@@ -2519,7 +2519,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
         <v>70</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="D46" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -2538,7 +2538,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
         <v>71</v>
       </c>
@@ -2557,7 +2557,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
         <v>72</v>
       </c>
@@ -2576,7 +2576,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
         <v>73</v>
       </c>
@@ -2595,7 +2595,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
         <v>74</v>
       </c>
@@ -2614,7 +2614,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
         <v>75</v>
       </c>
@@ -2633,7 +2633,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
         <v>76</v>
       </c>
@@ -2652,7 +2652,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
         <v>77</v>
       </c>
@@ -2671,7 +2671,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
         <v>78</v>
       </c>
@@ -2690,7 +2690,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
         <v>79</v>
       </c>
@@ -2709,7 +2709,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
         <v>80</v>
       </c>
@@ -2728,7 +2728,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
         <v>86</v>
       </c>
@@ -2747,19 +2747,11 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C58" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D58" s="1" t="b">
-        <v>0</v>
-      </c>
+    <row r="58" spans="1:9">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -2769,6 +2761,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2781,12 +2778,12 @@
       <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2815,7 +2812,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -2842,7 +2839,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2869,7 +2866,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -2896,7 +2893,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -2923,7 +2920,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -2950,7 +2947,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>81</v>
       </c>
@@ -2973,7 +2970,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>82</v>
       </c>
@@ -2992,7 +2989,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>83</v>
       </c>
@@ -3011,7 +3008,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>84</v>
       </c>
@@ -3030,7 +3027,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>85</v>
       </c>
@@ -3049,7 +3046,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -3076,7 +3073,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -3103,7 +3100,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -3132,7 +3129,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -3159,7 +3156,7 @@
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -3186,7 +3183,7 @@
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -3213,7 +3210,7 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -3240,7 +3237,7 @@
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -3267,7 +3264,7 @@
       </c>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -3294,7 +3291,7 @@
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -3321,7 +3318,7 @@
       </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -3348,7 +3345,7 @@
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -3375,7 +3372,7 @@
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -3402,7 +3399,7 @@
       </c>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -3431,7 +3428,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -3460,7 +3457,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -3487,7 +3484,7 @@
       </c>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -3516,7 +3513,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
@@ -3543,7 +3540,7 @@
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -3572,7 +3569,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -3599,7 +3596,7 @@
       </c>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -3626,7 +3623,7 @@
       </c>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -3653,7 +3650,7 @@
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
@@ -3680,7 +3677,7 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
@@ -3707,7 +3704,7 @@
       </c>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
         <v>60</v>
       </c>
@@ -3736,7 +3733,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
         <v>61</v>
       </c>
@@ -3763,7 +3760,7 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
@@ -3792,7 +3789,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
         <v>63</v>
       </c>
@@ -3821,7 +3818,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
         <v>64</v>
       </c>
@@ -3846,7 +3843,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
         <v>65</v>
       </c>
@@ -3871,7 +3868,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
         <v>66</v>
       </c>
@@ -3890,7 +3887,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
         <v>67</v>
       </c>
@@ -3909,7 +3906,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
         <v>68</v>
       </c>
@@ -3928,7 +3925,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
         <v>69</v>
       </c>
@@ -3947,7 +3944,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
         <v>70</v>
       </c>
@@ -3966,7 +3963,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
         <v>71</v>
       </c>
@@ -3985,7 +3982,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
         <v>72</v>
       </c>
@@ -4004,7 +4001,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
         <v>73</v>
       </c>
@@ -4023,7 +4020,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
         <v>74</v>
       </c>
@@ -4042,7 +4039,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
         <v>75</v>
       </c>
@@ -4061,7 +4058,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
         <v>76</v>
       </c>
@@ -4080,7 +4077,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
         <v>77</v>
       </c>
@@ -4099,7 +4096,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
         <v>78</v>
       </c>
@@ -4118,7 +4115,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
         <v>79</v>
       </c>
@@ -4137,7 +4134,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
         <v>80</v>
       </c>
@@ -4156,7 +4153,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
         <v>86</v>
       </c>
@@ -4175,7 +4172,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
         <v>87</v>
       </c>
@@ -4197,6 +4194,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4209,12 +4211,12 @@
       <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4243,7 +4245,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -4270,7 +4272,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -4297,7 +4299,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -4324,7 +4326,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -4351,7 +4353,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -4378,7 +4380,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>81</v>
       </c>
@@ -4401,7 +4403,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>82</v>
       </c>
@@ -4420,7 +4422,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>83</v>
       </c>
@@ -4439,7 +4441,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>84</v>
       </c>
@@ -4458,7 +4460,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>85</v>
       </c>
@@ -4477,7 +4479,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -4504,7 +4506,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -4531,7 +4533,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -4560,7 +4562,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -4587,7 +4589,7 @@
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -4614,7 +4616,7 @@
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -4641,7 +4643,7 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -4668,7 +4670,7 @@
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -4695,7 +4697,7 @@
       </c>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -4722,7 +4724,7 @@
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -4749,7 +4751,7 @@
       </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -4776,7 +4778,7 @@
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -4803,7 +4805,7 @@
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -4830,7 +4832,7 @@
       </c>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -4859,7 +4861,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -4888,7 +4890,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -4915,7 +4917,7 @@
       </c>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -4944,7 +4946,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
@@ -4971,7 +4973,7 @@
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -5000,7 +5002,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -5027,7 +5029,7 @@
       </c>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -5054,7 +5056,7 @@
       </c>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -5081,7 +5083,7 @@
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
@@ -5108,7 +5110,7 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
@@ -5135,7 +5137,7 @@
       </c>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
         <v>60</v>
       </c>
@@ -5164,7 +5166,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
         <v>61</v>
       </c>
@@ -5191,7 +5193,7 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
@@ -5220,7 +5222,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
         <v>63</v>
       </c>
@@ -5249,7 +5251,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
         <v>64</v>
       </c>
@@ -5274,7 +5276,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
         <v>65</v>
       </c>
@@ -5299,7 +5301,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
         <v>66</v>
       </c>
@@ -5318,7 +5320,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
         <v>67</v>
       </c>
@@ -5337,7 +5339,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
         <v>68</v>
       </c>
@@ -5356,7 +5358,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
         <v>69</v>
       </c>
@@ -5375,7 +5377,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
         <v>70</v>
       </c>
@@ -5394,7 +5396,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
         <v>71</v>
       </c>
@@ -5413,7 +5415,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
         <v>72</v>
       </c>
@@ -5432,7 +5434,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
         <v>73</v>
       </c>
@@ -5451,7 +5453,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
         <v>74</v>
       </c>
@@ -5470,7 +5472,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
         <v>75</v>
       </c>
@@ -5489,7 +5491,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
         <v>76</v>
       </c>
@@ -5508,7 +5510,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
         <v>77</v>
       </c>
@@ -5527,7 +5529,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
         <v>78</v>
       </c>
@@ -5546,7 +5548,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
         <v>79</v>
       </c>
@@ -5565,7 +5567,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
         <v>80</v>
       </c>
@@ -5584,7 +5586,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
         <v>86</v>
       </c>
@@ -5603,7 +5605,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
         <v>87</v>
       </c>
@@ -5625,5 +5627,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed certain demos from CellOrganizer Version 2.8.0
</commit_message>
<xml_diff>
--- a/demo_lists.xlsx
+++ b/demo_lists.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/piepi/CellOrganizer/cellorganizer-docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matamala/Documents/MATLAB/cellorganizer-docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6193B453-8AFB-844C-AF78-84739EB0E536}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v2.8.0" sheetId="6" r:id="rId1"/>
@@ -20,10 +21,15 @@
     <sheet name="v2.7.0" sheetId="3" r:id="rId5"/>
     <sheet name="v2.6" sheetId="2" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -344,7 +350,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -662,12 +668,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F69" sqref="F69"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -748,7 +754,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -767,7 +773,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -786,16 +792,16 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -805,7 +811,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -824,16 +830,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -843,7 +849,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
@@ -862,16 +868,16 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -881,7 +887,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>14</v>
@@ -900,7 +906,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
@@ -909,7 +915,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -919,7 +925,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
@@ -928,7 +934,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -938,7 +944,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>14</v>
@@ -957,7 +963,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>14</v>
@@ -976,7 +982,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>14</v>
@@ -995,7 +1001,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>14</v>
@@ -1014,7 +1020,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>14</v>
@@ -1033,16 +1039,16 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1052,16 +1058,16 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -1071,7 +1077,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>14</v>
@@ -1080,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1090,13 +1096,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1" t="b">
         <v>0</v>
@@ -1109,16 +1115,16 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1128,7 +1134,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>14</v>
@@ -1147,7 +1153,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>14</v>
@@ -1166,16 +1172,16 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -1185,7 +1191,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>14</v>
@@ -1194,7 +1200,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -1204,16 +1210,16 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C29" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1223,7 +1229,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>14</v>
@@ -1232,7 +1238,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -1242,13 +1248,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" s="1" t="b">
         <v>0</v>
@@ -1261,7 +1267,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>14</v>
@@ -1280,7 +1286,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>14</v>
@@ -1299,7 +1305,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>14</v>
@@ -1318,7 +1324,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>14</v>
@@ -1337,7 +1343,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>14</v>
@@ -1356,7 +1362,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>14</v>
@@ -1365,7 +1371,7 @@
         <v>0</v>
       </c>
       <c r="D37" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -1375,7 +1381,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>14</v>
@@ -1384,7 +1390,7 @@
         <v>0</v>
       </c>
       <c r="D38" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -1394,7 +1400,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>14</v>
@@ -1403,7 +1409,7 @@
         <v>0</v>
       </c>
       <c r="D39" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -1413,16 +1419,16 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C40" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -1432,7 +1438,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>14</v>
@@ -1451,16 +1457,16 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C42" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -1470,7 +1476,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>14</v>
@@ -1489,16 +1495,16 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C44" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -1508,7 +1514,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>14</v>
@@ -1527,7 +1533,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>14</v>
@@ -1536,7 +1542,7 @@
         <v>0</v>
       </c>
       <c r="D46" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -1546,16 +1552,16 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C47" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -1565,7 +1571,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>14</v>
@@ -1584,7 +1590,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>14</v>
@@ -1593,7 +1599,7 @@
         <v>0</v>
       </c>
       <c r="D49" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -1603,26 +1609,21 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C50" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>14</v>
@@ -1633,34 +1634,24 @@
       <c r="D51" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C52" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>14</v>
@@ -1671,15 +1662,10 @@
       <c r="D53" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>14</v>
@@ -1688,17 +1674,12 @@
         <v>0</v>
       </c>
       <c r="D54" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>14</v>
@@ -1707,17 +1688,12 @@
         <v>0</v>
       </c>
       <c r="D55" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>14</v>
@@ -1728,15 +1704,10 @@
       <c r="D56" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>14</v>
@@ -1747,15 +1718,10 @@
       <c r="D57" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>14</v>
@@ -1766,21 +1732,16 @@
       <c r="D58" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C59" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59" s="1" t="b">
         <v>0</v>
@@ -1788,21 +1749,21 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C60" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>14</v>
@@ -1816,7 +1777,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>14</v>
@@ -1825,132 +1786,6 @@
         <v>1</v>
       </c>
       <c r="D62" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C63" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D63" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C64" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D64" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C65" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D65" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C66" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D66" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C67" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D67" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C68" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D68" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C69" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D69" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C70" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D70" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C71" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D71" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1960,7 +1795,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView windowProtection="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
@@ -2997,7 +2832,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView windowProtection="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
@@ -4105,7 +3940,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView windowProtection="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
@@ -5213,7 +5048,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView windowProtection="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
@@ -6640,7 +6475,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView windowProtection="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">

</xml_diff>

<commit_message>
Resolve "Add Singularity section"
</commit_message>
<xml_diff>
--- a/demo_lists.xlsx
+++ b/demo_lists.xlsx
@@ -1,36 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matamala/Documents/MATLAB/cellorganizer-docs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6193B453-8AFB-844C-AF78-84739EB0E536}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14120" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="v2.8.0" sheetId="6" r:id="rId1"/>
-    <sheet name="v2.5" sheetId="1" r:id="rId2"/>
+    <sheet name="v2.5" sheetId="1" r:id="rId1"/>
+    <sheet name="v2.8.0" sheetId="6" r:id="rId2"/>
     <sheet name="v2.7.2" sheetId="5" r:id="rId3"/>
     <sheet name="v2.7.1" sheetId="4" r:id="rId4"/>
     <sheet name="v2.7.0" sheetId="3" r:id="rId5"/>
     <sheet name="v2.6" sheetId="2" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -42,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -306,51 +292,12 @@
   </si>
   <si>
     <t>demo3D47</t>
-  </si>
-  <si>
-    <t>demo3D48</t>
-  </si>
-  <si>
-    <t>demo3D49</t>
-  </si>
-  <si>
-    <t>demo3D50</t>
-  </si>
-  <si>
-    <t>demo3D51</t>
-  </si>
-  <si>
-    <t>demo3D52</t>
-  </si>
-  <si>
-    <t>demo3D53</t>
-  </si>
-  <si>
-    <t>demo3D54</t>
-  </si>
-  <si>
-    <t>demo3D55</t>
-  </si>
-  <si>
-    <t>demo3D56</t>
-  </si>
-  <si>
-    <t>demo3D57</t>
-  </si>
-  <si>
-    <t>demo3D58</t>
-  </si>
-  <si>
-    <t>demo3D59</t>
-  </si>
-  <si>
-    <t>demo3D60</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -661,1141 +608,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I62"/>
-  <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33:XFD33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D24" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D30" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D31" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D32" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D33" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D34" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D35" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D36" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D37" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D38" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D39" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D40" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D41" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D42" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D43" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D44" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D45" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C46" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D46" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D47" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D48" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C49" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D49" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D50" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C51" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D51" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C52" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D52" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C53" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D53" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C54" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D54" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C55" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D55" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C56" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D56" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C57" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D57" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C58" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D58" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C59" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D59" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C60" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D60" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C61" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D61" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C62" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D62" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView windowProtection="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
@@ -1803,9 +623,9 @@
       <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1828,7 +648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1856,7 +676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1884,7 +704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1912,7 +732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1940,7 +760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1968,7 +788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1996,7 +816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2024,7 +844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2052,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2080,7 +900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2108,7 +928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2136,7 +956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2164,7 +984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2192,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2220,7 +1040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2248,7 +1068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2276,7 +1096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2304,7 +1124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2332,7 +1152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -2360,7 +1180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -2388,7 +1208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -2416,7 +1236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -2444,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -2472,7 +1292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -2500,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -2528,7 +1348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2556,7 +1376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -2584,7 +1404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -2612,7 +1432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -2640,7 +1460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -2668,7 +1488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -2696,7 +1516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -2724,7 +1544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -2752,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -2780,7 +1600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -2803,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -2828,24 +1648,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView windowProtection="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2859,7 +1684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -2878,7 +1703,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2897,7 +1722,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -2916,7 +1741,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -2935,7 +1760,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -2954,7 +1779,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>81</v>
       </c>
@@ -2973,7 +1798,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>82</v>
       </c>
@@ -2992,7 +1817,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>83</v>
       </c>
@@ -3011,7 +1836,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>84</v>
       </c>
@@ -3030,7 +1855,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>85</v>
       </c>
@@ -3049,7 +1874,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -3068,7 +1893,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -3087,7 +1912,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -3106,7 +1931,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -3125,7 +1950,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -3144,7 +1969,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -3163,7 +1988,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -3182,7 +2007,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -3201,7 +2026,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -3220,7 +2045,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -3239,7 +2064,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -3258,7 +2083,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -3277,7 +2102,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -3296,7 +2121,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -3315,7 +2140,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -3334,7 +2159,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -3353,7 +2178,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -3372,7 +2197,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
@@ -3391,7 +2216,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -3410,7 +2235,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -3429,7 +2254,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -3448,7 +2273,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -3467,7 +2292,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
@@ -3486,7 +2311,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
@@ -3505,7 +2330,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
         <v>60</v>
       </c>
@@ -3524,7 +2349,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
         <v>61</v>
       </c>
@@ -3543,7 +2368,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
@@ -3562,7 +2387,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
         <v>63</v>
       </c>
@@ -3581,7 +2406,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
         <v>64</v>
       </c>
@@ -3600,7 +2425,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
         <v>65</v>
       </c>
@@ -3619,7 +2444,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
         <v>66</v>
       </c>
@@ -3638,7 +2463,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
         <v>67</v>
       </c>
@@ -3657,7 +2482,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
         <v>68</v>
       </c>
@@ -3676,7 +2501,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
         <v>69</v>
       </c>
@@ -3695,7 +2520,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
         <v>70</v>
       </c>
@@ -3714,7 +2539,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
         <v>71</v>
       </c>
@@ -3733,7 +2558,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
         <v>72</v>
       </c>
@@ -3752,7 +2577,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
         <v>73</v>
       </c>
@@ -3771,7 +2596,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
         <v>74</v>
       </c>
@@ -3790,7 +2615,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
         <v>75</v>
       </c>
@@ -3809,7 +2634,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
         <v>76</v>
       </c>
@@ -3828,7 +2653,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
         <v>77</v>
       </c>
@@ -3847,7 +2672,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
         <v>78</v>
       </c>
@@ -3866,7 +2691,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
         <v>79</v>
       </c>
@@ -3885,7 +2710,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
         <v>80</v>
       </c>
@@ -3904,7 +2729,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
         <v>86</v>
       </c>
@@ -3923,7 +2748,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -3936,11 +2761,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView windowProtection="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
@@ -3948,12 +2778,12 @@
       <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3967,7 +2797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -3986,7 +2816,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -4005,7 +2835,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -4024,7 +2854,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -4043,7 +2873,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -4062,7 +2892,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>81</v>
       </c>
@@ -4081,7 +2911,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>82</v>
       </c>
@@ -4100,7 +2930,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>83</v>
       </c>
@@ -4119,7 +2949,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>84</v>
       </c>
@@ -4138,7 +2968,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>85</v>
       </c>
@@ -4157,7 +2987,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -4176,7 +3006,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -4195,7 +3025,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -4214,7 +3044,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -4233,7 +3063,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -4252,7 +3082,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -4271,7 +3101,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -4290,7 +3120,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -4309,7 +3139,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -4328,7 +3158,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -4347,7 +3177,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -4366,7 +3196,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -4385,7 +3215,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -4404,7 +3234,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -4423,7 +3253,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -4442,7 +3272,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -4461,7 +3291,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -4480,7 +3310,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
@@ -4499,7 +3329,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -4518,7 +3348,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -4537,7 +3367,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -4556,7 +3386,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -4575,7 +3405,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
@@ -4594,7 +3424,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
@@ -4613,7 +3443,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
         <v>60</v>
       </c>
@@ -4632,7 +3462,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
         <v>61</v>
       </c>
@@ -4651,7 +3481,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
@@ -4670,7 +3500,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
         <v>63</v>
       </c>
@@ -4689,7 +3519,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
         <v>64</v>
       </c>
@@ -4708,7 +3538,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
         <v>65</v>
       </c>
@@ -4727,7 +3557,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
         <v>66</v>
       </c>
@@ -4746,7 +3576,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
         <v>67</v>
       </c>
@@ -4765,7 +3595,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
         <v>68</v>
       </c>
@@ -4784,7 +3614,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
         <v>69</v>
       </c>
@@ -4803,7 +3633,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
         <v>70</v>
       </c>
@@ -4822,7 +3652,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
         <v>71</v>
       </c>
@@ -4841,7 +3671,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
         <v>72</v>
       </c>
@@ -4860,7 +3690,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
         <v>73</v>
       </c>
@@ -4879,7 +3709,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
         <v>74</v>
       </c>
@@ -4898,7 +3728,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
         <v>75</v>
       </c>
@@ -4917,7 +3747,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
         <v>76</v>
       </c>
@@ -4936,7 +3766,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
         <v>77</v>
       </c>
@@ -4955,7 +3785,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
         <v>78</v>
       </c>
@@ -4974,7 +3804,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
         <v>79</v>
       </c>
@@ -4993,7 +3823,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
         <v>80</v>
       </c>
@@ -5012,7 +3842,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
         <v>86</v>
       </c>
@@ -5031,7 +3861,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -5044,11 +3874,1129 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I58"/>
+  <sheetViews>
+    <sheetView windowProtection="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D53" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D56" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView windowProtection="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
@@ -5056,12 +5004,12 @@
       <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5090,7 +5038,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -5117,7 +5065,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -5144,7 +5092,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -5171,7 +5119,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -5198,7 +5146,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -5225,7 +5173,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>81</v>
       </c>
@@ -5248,7 +5196,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>82</v>
       </c>
@@ -5267,7 +5215,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>83</v>
       </c>
@@ -5286,7 +5234,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>84</v>
       </c>
@@ -5305,7 +5253,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>85</v>
       </c>
@@ -5324,7 +5272,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -5351,7 +5299,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -5378,7 +5326,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -5407,7 +5355,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -5434,7 +5382,7 @@
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -5461,7 +5409,7 @@
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -5488,7 +5436,7 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -5515,7 +5463,7 @@
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -5542,7 +5490,7 @@
       </c>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -5569,7 +5517,7 @@
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -5596,7 +5544,7 @@
       </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -5623,7 +5571,7 @@
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -5650,7 +5598,7 @@
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -5677,7 +5625,7 @@
       </c>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -5706,7 +5654,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -5735,7 +5683,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -5762,7 +5710,7 @@
       </c>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -5791,7 +5739,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
@@ -5818,7 +5766,7 @@
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -5847,7 +5795,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -5874,7 +5822,7 @@
       </c>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -5901,7 +5849,7 @@
       </c>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -5928,7 +5876,7 @@
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
@@ -5955,7 +5903,7 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
@@ -5982,7 +5930,7 @@
       </c>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
         <v>60</v>
       </c>
@@ -6011,7 +5959,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
         <v>61</v>
       </c>
@@ -6038,7 +5986,7 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
@@ -6067,7 +6015,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
         <v>63</v>
       </c>
@@ -6096,7 +6044,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
         <v>64</v>
       </c>
@@ -6121,7 +6069,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
         <v>65</v>
       </c>
@@ -6146,7 +6094,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
         <v>66</v>
       </c>
@@ -6165,7 +6113,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
         <v>67</v>
       </c>
@@ -6184,7 +6132,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
         <v>68</v>
       </c>
@@ -6203,7 +6151,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
         <v>69</v>
       </c>
@@ -6222,7 +6170,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
         <v>70</v>
       </c>
@@ -6241,7 +6189,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
         <v>71</v>
       </c>
@@ -6260,7 +6208,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
         <v>72</v>
       </c>
@@ -6279,7 +6227,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
         <v>73</v>
       </c>
@@ -6298,7 +6246,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
         <v>74</v>
       </c>
@@ -6317,7 +6265,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
         <v>75</v>
       </c>
@@ -6336,7 +6284,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
         <v>76</v>
       </c>
@@ -6355,7 +6303,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
         <v>77</v>
       </c>
@@ -6374,7 +6322,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
         <v>78</v>
       </c>
@@ -6393,7 +6341,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
         <v>79</v>
       </c>
@@ -6412,7 +6360,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
         <v>80</v>
       </c>
@@ -6431,7 +6379,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
         <v>86</v>
       </c>
@@ -6450,7 +6398,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
         <v>87</v>
       </c>
@@ -6471,11 +6419,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView windowProtection="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
@@ -6483,12 +6436,12 @@
       <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6517,7 +6470,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -6544,7 +6497,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -6571,7 +6524,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -6598,7 +6551,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -6625,7 +6578,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -6652,7 +6605,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>81</v>
       </c>
@@ -6675,7 +6628,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>82</v>
       </c>
@@ -6694,7 +6647,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>83</v>
       </c>
@@ -6713,7 +6666,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>84</v>
       </c>
@@ -6732,7 +6685,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>85</v>
       </c>
@@ -6751,7 +6704,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -6778,7 +6731,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -6805,7 +6758,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -6834,7 +6787,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -6861,7 +6814,7 @@
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -6888,7 +6841,7 @@
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -6915,7 +6868,7 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -6942,7 +6895,7 @@
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -6969,7 +6922,7 @@
       </c>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -6996,7 +6949,7 @@
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -7023,7 +6976,7 @@
       </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -7050,7 +7003,7 @@
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -7077,7 +7030,7 @@
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -7104,7 +7057,7 @@
       </c>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -7133,7 +7086,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -7162,7 +7115,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -7189,7 +7142,7 @@
       </c>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -7218,7 +7171,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
@@ -7245,7 +7198,7 @@
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -7274,7 +7227,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -7301,7 +7254,7 @@
       </c>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -7328,7 +7281,7 @@
       </c>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -7355,7 +7308,7 @@
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
@@ -7382,7 +7335,7 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
@@ -7409,7 +7362,7 @@
       </c>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
         <v>60</v>
       </c>
@@ -7438,7 +7391,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
         <v>61</v>
       </c>
@@ -7465,7 +7418,7 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
@@ -7494,7 +7447,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
         <v>63</v>
       </c>
@@ -7523,7 +7476,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
         <v>64</v>
       </c>
@@ -7548,7 +7501,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
         <v>65</v>
       </c>
@@ -7573,7 +7526,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
         <v>66</v>
       </c>
@@ -7592,7 +7545,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
         <v>67</v>
       </c>
@@ -7611,7 +7564,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
         <v>68</v>
       </c>
@@ -7630,7 +7583,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
         <v>69</v>
       </c>
@@ -7649,7 +7602,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
         <v>70</v>
       </c>
@@ -7668,7 +7621,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
         <v>71</v>
       </c>
@@ -7687,7 +7640,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
         <v>72</v>
       </c>
@@ -7706,7 +7659,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
         <v>73</v>
       </c>
@@ -7725,7 +7678,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
         <v>74</v>
       </c>
@@ -7744,7 +7697,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
         <v>75</v>
       </c>
@@ -7763,7 +7716,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
         <v>76</v>
       </c>
@@ -7782,7 +7735,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
         <v>77</v>
       </c>
@@ -7801,7 +7754,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
         <v>78</v>
       </c>
@@ -7820,7 +7773,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
         <v>79</v>
       </c>
@@ -7839,7 +7792,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
         <v>80</v>
       </c>
@@ -7858,7 +7811,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
         <v>86</v>
       </c>
@@ -7877,7 +7830,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
         <v>87</v>
       </c>
@@ -7898,5 +7851,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>